<commit_message>
Finish 13 new test scrtips
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TestScripts.xlsx
+++ b/NformTester/NformTester/keywordscripts/TestScripts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16035" windowHeight="12720"/>
@@ -1352,7 +1352,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8179" uniqueCount="928">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8178" uniqueCount="928">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -4168,7 +4168,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$Sys_TestObject_NformViewer$</t>
+    <t>$DB_Test$</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -4690,7 +4690,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4787,9 +4787,7 @@
       <c r="F3" s="4" t="s">
         <v>927</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>925</v>
-      </c>
+      <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>

</xml_diff>